<commit_message>
REady for testrun of BABY_model_LOO_enchilada -- performs regressions only if correct numbers of NDs
</commit_message>
<xml_diff>
--- a/INDIV_MODELS/Regression_double_check.xlsx
+++ b/INDIV_MODELS/Regression_double_check.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15700" windowHeight="16600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26500" windowHeight="15840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -50,12 +50,6 @@
   </si>
   <si>
     <t>SpC_EVENT</t>
-  </si>
-  <si>
-    <t>intercept</t>
-  </si>
-  <si>
-    <t>slope</t>
   </si>
 </sst>
 </file>
@@ -104,8 +98,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -172,7 +172,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="69">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -204,6 +204,9 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -235,6 +238,9 @@
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -272,17 +278,8 @@
           </c:spPr>
           <c:trendline>
             <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.265818460192476"/>
-                  <c:y val="-0.181952099737533"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -394,10 +391,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.901956</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.269956</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -412,11 +409,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="539427768"/>
-        <c:axId val="539430664"/>
+        <c:axId val="601094152"/>
+        <c:axId val="601097144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="539427768"/>
+        <c:axId val="601094152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -426,12 +423,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="539430664"/>
+        <c:crossAx val="601097144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="539430664"/>
+        <c:axId val="601097144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="4.0"/>
@@ -443,7 +440,136 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="539427768"/>
+        <c:crossAx val="601094152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$45:$E$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2.34648895767015</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.557491404004623</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$46:$E$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2.732422697420184</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.994072213796786</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="605994952"/>
+        <c:axId val="605991784"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="605994952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="605991784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="605991784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="605994952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -492,6 +618,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>692150</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -822,9 +978,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E46" sqref="D45:E46"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
@@ -1231,7 +1389,7 @@
         <v>4.5108595065168497</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="4:5">
       <c r="D17">
         <f t="shared" si="2"/>
         <v>2.9301265164559971</v>
@@ -1241,7 +1399,7 @@
         <v>4.8751973232011512</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="4:5">
       <c r="D18">
         <f t="shared" si="2"/>
         <v>2.9507349076232554</v>
@@ -1251,7 +1409,7 @@
         <v>5.1984970312658261</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="4:5">
       <c r="D19">
         <f t="shared" si="2"/>
         <v>3.0301337002713233</v>
@@ -1261,7 +1419,7 @@
         <v>5.2522734280466299</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="4:5">
       <c r="D20">
         <f t="shared" si="2"/>
         <v>2.8419981736119486</v>
@@ -1271,7 +1429,7 @@
         <v>5.3518581334760666</v>
       </c>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="4:5">
       <c r="D21">
         <f t="shared" si="2"/>
         <v>3.0487989944906833</v>
@@ -1281,7 +1439,7 @@
         <v>5.4847969334906548</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="4:5">
       <c r="D22">
         <f t="shared" si="2"/>
         <v>2.9301265164559971</v>
@@ -1291,34 +1449,104 @@
         <v>5.5645204073226937</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
-      <c r="B25" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25">
-        <v>0.90195599999999998</v>
-      </c>
+    <row r="25" spans="4:5">
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
         <f>D25*C26+C25</f>
-        <v>0.90195599999999998</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5">
-      <c r="B26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26">
-        <v>7.0919999999999996</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="4:5">
       <c r="D26">
         <v>4</v>
       </c>
       <c r="E26">
         <f>D26*C26+C25</f>
-        <v>29.269955999999997</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41">
+        <v>320</v>
+      </c>
+      <c r="B41">
+        <v>19</v>
+      </c>
+      <c r="C41">
+        <v>9.4488190000000003</v>
+      </c>
+      <c r="D41">
+        <f>LN(C41+1)</f>
+        <v>2.3464889576701498</v>
+      </c>
+      <c r="E41">
+        <v>9.4343999999999997E-2</v>
+      </c>
+      <c r="F41">
+        <f>LN((E41*1000)+1)</f>
+        <v>4.5574914040046233</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>25192</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42">
+        <v>320</v>
+      </c>
+      <c r="B42">
+        <v>19</v>
+      </c>
+      <c r="C42">
+        <v>14.370079</v>
+      </c>
+      <c r="D42">
+        <f>LN(C42+1)</f>
+        <v>2.732422697420184</v>
+      </c>
+      <c r="E42">
+        <v>0.146536</v>
+      </c>
+      <c r="F42">
+        <f>LN((E42*1000)+1)</f>
+        <v>4.9940722137967857</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>25193</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="D45">
+        <f>D41</f>
+        <v>2.3464889576701498</v>
+      </c>
+      <c r="E45">
+        <f>F41</f>
+        <v>4.5574914040046233</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="D46">
+        <f>D42</f>
+        <v>2.732422697420184</v>
+      </c>
+      <c r="E46">
+        <f>F42</f>
+        <v>4.9940722137967857</v>
       </c>
     </row>
   </sheetData>
@@ -1337,7 +1565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -1581,7 +1809,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>